<commit_message>
LR all window & Voting+ W1,2
</commit_message>
<xml_diff>
--- a/data/performance_sheets_option2/window1/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets_option2/window1/BA11 Overall Model Peformance Results.xlsx
@@ -770,19 +770,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.03302307327921955</v>
+        <v>0.02460305133102218</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1579703957948224</v>
+        <v>0.1335624111428828</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.2369622940602663</v>
+        <v>0.3295153988291273</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.1817225172597484</v>
+        <v>0.1568535983999799</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>27.26329154366778</v>
+        <v>25.76434697848138</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -800,19 +800,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.03929773636754546</v>
+        <v>0.02374431203525316</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.171329634287022</v>
+        <v>0.128863541725167</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.2439569531004755</v>
+        <v>0.3498250725560305</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1982365666761444</v>
+        <v>0.1540918947746868</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>28.74078468498735</v>
+        <v>24.97633857941893</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -1158,23 +1158,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.03341064842908602</v>
+        <v>0.01675042928639316</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1382051149702713</v>
+        <v>0.1007609123326643</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1885355638377754</v>
+        <v>0.3366699586023007</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1827857993091532</v>
+        <v>0.1294234495228479</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>21.88757235384928</v>
+        <v>20.32247934875175</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -1188,23 +1188,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.0368108745961055</v>
+        <v>0.01722504582272745</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1503964037111316</v>
+        <v>0.1016792560404173</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.212278645817269</v>
+        <v>0.346825073109033</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1918616027143146</v>
+        <v>0.1312442220546392</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>24.10112997270878</v>
+        <v>20.56211707445415</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -1224,19 +1224,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.0516799366631526</v>
+        <v>0.02752271227816009</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1689330188328717</v>
+        <v>0.1251832398323845</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.34625148435272</v>
+        <v>0.4397310940709978</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2273322165095669</v>
+        <v>0.1658997054794254</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>26.34952887275096</v>
+        <v>23.89769575540419</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -1254,19 +1254,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.05636122196412943</v>
+        <v>0.02931804448191932</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1821553983477377</v>
+        <v>0.1251437690345378</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.364111882688522</v>
+        <v>0.4747263690140186</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2374051852090207</v>
+        <v>0.1712251280680477</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>28.47915455819305</v>
+        <v>23.96385610795175</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -1282,23 +1282,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.05271306615882325</v>
+        <v>0.02247836288648006</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1732552169619059</v>
+        <v>0.1150116612066147</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.3235760813201814</v>
+        <v>0.3666019861389967</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2295932624421354</v>
+        <v>0.149927858940492</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>27.05428344221931</v>
+        <v>22.26891798804478</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -1312,23 +1312,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.04890990680929479</v>
+        <v>0.02373192107638142</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1716856340344498</v>
+        <v>0.1073421699748295</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.3145978507633219</v>
+        <v>0.375668788374639</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2211558428106633</v>
+        <v>0.1540516831338802</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>26.82382863326954</v>
+        <v>21.22219926564155</v>
       </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
@@ -2085,19 +2085,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>6.118568609350986e-07</v>
+        <v>0.3696887468630021</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0006199100350023499</v>
+        <v>0.4935428647316564</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.0003081258115772942</v>
+        <v>0.2606866773231619</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.0007822127977316011</v>
+        <v>0.6080203506980685</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.03079814301146308</v>
+        <v>21.28584873235279</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -2115,19 +2115,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>4.456985851372211e-07</v>
+        <v>0.3569773175454626</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.0005302893508958317</v>
+        <v>0.48920498528044</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.0002629039582065132</v>
+        <v>0.2554978896338939</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.0006676066095667576</v>
+        <v>0.5974757882504216</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.02628052423642991</v>
+        <v>21.48146456111527</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -2477,19 +2477,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.4837106163782679</v>
+        <v>1.102887416715771</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.6126891633185556</v>
+        <v>0.9335372062922906</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.2470062202783311</v>
+        <v>0.4556491055429305</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.6954930742849047</v>
+        <v>1.050184467946356</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>28.02398405917912</v>
+        <v>45.1715029928123</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -2503,23 +2503,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>1.083876832350345</v>
+        <v>0.5049336988670124</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.9686296298130519</v>
+        <v>0.549525976335083</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.375193397506086</v>
+        <v>0.3286723682158204</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>1.041094055477383</v>
+        <v>0.7105868693319716</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>45.25118228871472</v>
+        <v>26.38389273368112</v>
       </c>
     </row>
     <row r="14">
@@ -2539,19 +2539,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.8521792109133791</v>
+        <v>0.8793356050812787</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.7907128706148484</v>
+        <v>0.5630837950887423</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.41012039803817</v>
+        <v>0.488824894377403</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.9231355322558975</v>
+        <v>0.9377289614175722</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>35.06315436075247</v>
+        <v>24.41232243259562</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -2565,23 +2565,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>1.561735876901704</v>
+        <v>0.4288462494677742</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>1.124206494545019</v>
+        <v>0.3954669189234346</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.5680564451136172</v>
+        <v>0.3538620532904961</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>1.249694313382958</v>
+        <v>0.6548635349962419</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>51.96992117707736</v>
+        <v>18.73455700727488</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -2601,19 +2601,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.3745969813141874</v>
+        <v>0.4339195350240614</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.4764403042675752</v>
+        <v>0.5481053087253319</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.280817195930726</v>
+        <v>0.3606608092560575</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.6120432838567771</v>
+        <v>0.6587256902718016</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>21.01166117868811</v>
+        <v>25.40731012375008</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -2631,19 +2631,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.4072507134030361</v>
+        <v>0.4420279850935904</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.4876189738060278</v>
+        <v>0.5116333169850067</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2954852345266354</v>
+        <v>0.3659115711837184</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.6381619805371017</v>
+        <v>0.6648518519892912</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>21.34822560678776</v>
+        <v>23.66982733769425</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -3397,19 +3397,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>2.663596121388047e-07</v>
+        <v>0.3972327646529404</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0004273137947934234</v>
+        <v>0.538683781189665</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.0001985783687981264</v>
+        <v>0.2611857523445343</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.0005161003895937347</v>
+        <v>0.6302640435983481</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.01985258226288783</v>
+        <v>22.70539600542244</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -3427,19 +3427,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>2.235244822285724e-07</v>
+        <v>0.4002497423604819</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.0003825669571935753</v>
+        <v>0.5404074057063895</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.0001711021235415052</v>
+        <v>0.2651519088404322</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.0004727837584229944</v>
+        <v>0.6326529398971302</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.01710665990867106</v>
+        <v>23.60441176630317</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -3789,19 +3789,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.4345546882368168</v>
+        <v>0.7088846633838815</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.5900744543700709</v>
+        <v>0.7057959629600908</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.2354434960031143</v>
+        <v>0.2912970843966241</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.6592076214947888</v>
+        <v>0.841952886677088</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>26.13104761365046</v>
+        <v>32.88548784117884</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -3815,23 +3815,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.4794937026739445</v>
+        <v>0.9510379281879265</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.6156453858022384</v>
+        <v>0.8946991996430309</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2408475496385665</v>
+        <v>0.3998917352510349</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.6924548380031325</v>
+        <v>0.9752117350544581</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>26.44034702035754</v>
+        <v>43.58957904087698</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -3851,19 +3851,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.2144526518025892</v>
+        <v>0.5318283562969249</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.3141304488443115</v>
+        <v>0.5884620639712925</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1918523247738438</v>
+        <v>0.3507905721220041</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.463090327908702</v>
+        <v>0.7292656280786343</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>13.55449026919958</v>
+        <v>26.18833125966283</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -3877,23 +3877,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.7459076885895907</v>
+        <v>0.5487420067531871</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.7232519802996272</v>
+        <v>0.6311954715397279</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.3519569845818983</v>
+        <v>0.3668886698613254</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.8636594749029218</v>
+        <v>0.7407712243015296</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>30.62652720291618</v>
+        <v>28.22207865106365</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -3913,19 +3913,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.3776332242584215</v>
+        <v>0.4099198988177201</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.5126170425795232</v>
+        <v>0.4819081590636137</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2465088582879834</v>
+        <v>0.31098425580037</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.6145186931724872</v>
+        <v>0.6402498721731384</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>21.78726292744672</v>
+        <v>21.66276240917403</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -3943,19 +3943,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.3168058384402216</v>
+        <v>0.5215198039370122</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.4653295406880977</v>
+        <v>0.6017459549770129</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2331582437945676</v>
+        <v>0.3531326751716206</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.5628550776534059</v>
+        <v>0.7221632806623529</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>19.74399893897817</v>
+        <v>26.88774191638504</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -4709,19 +4709,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>8.43510289174328e-07</v>
+        <v>0.1880071778580721</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0008030629392802544</v>
+        <v>0.3302397349943615</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.000304874973374408</v>
+        <v>0.1400046212870437</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.00091842816222845</v>
+        <v>0.4335979449421689</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.03049129166480794</v>
+        <v>16.04578681579047</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -4739,19 +4739,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>8.587424733664748e-07</v>
+        <v>0.1515941296510085</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.0007879175300604186</v>
+        <v>0.3171182581556938</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.0002987845778322083</v>
+        <v>0.1307538781048453</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.0009266835885923926</v>
+        <v>0.3893509081163269</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.02988259420151843</v>
+        <v>13.55835430926481</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -5097,23 +5097,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1.00471101887801</v>
+        <v>1.262926297077078</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.8826811330653667</v>
+        <v>1.049505991212684</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.3194788332254313</v>
+        <v>0.3947866918885353</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>1.002352741742152</v>
+        <v>1.123799936410871</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>39.731786626052</v>
+        <v>49.80068514307837</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -5127,23 +5127,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.4273629861840522</v>
+        <v>1.094564154123878</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.6025844643010891</v>
+        <v>0.8771903255863159</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2225442102819787</v>
+        <v>0.3305008251414246</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.6537300560507006</v>
+        <v>1.046214200880431</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>24.78390072631244</v>
+        <v>41.51639392408873</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -5163,19 +5163,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.0001398578752526366</v>
+        <v>0.5107861543452212</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.0109214063712496</v>
+        <v>0.4268239615216992</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.003914246116135152</v>
+        <v>0.3253091229000773</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.01182615217442413</v>
+        <v>0.7146930490393909</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>0.3905425109376747</v>
+        <v>18.13749370331966</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -5193,19 +5193,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.03200709416774628</v>
+        <v>0.5195650920718468</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1378651986628733</v>
+        <v>0.5262190727504213</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.06164389506839357</v>
+        <v>0.331279491873587</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.1789052659027852</v>
+        <v>0.7208086376229454</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>5.76417808455167</v>
+        <v>22.76917467230794</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -5225,19 +5225,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>2.242059683134919</v>
+        <v>2.040191999841351</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>1.360343800284332</v>
+        <v>1.217289740458477</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.4938811422526252</v>
+        <v>0.5493365871539327</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>1.497350888447634</v>
+        <v>1.428352897515649</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>71.01777628850472</v>
+        <v>69.92543991073069</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -5251,23 +5251,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.3817032916275601</v>
+        <v>2.993167359407795</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.5244280110124394</v>
+        <v>1.43367994903035</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2048537006043145</v>
+        <v>0.5619127255693618</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.6178214075504022</v>
+        <v>1.730077269779531</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>21.16937664622396</v>
+        <v>81.9436430306561</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -6019,19 +6019,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.05366659031406032</v>
+        <v>0.03184084281089721</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1581235911667858</v>
+        <v>0.1468975787836911</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.814795422212077</v>
+        <v>0.3841230597408987</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2316605065911329</v>
+        <v>0.1784400258095061</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>32.74590146894623</v>
+        <v>28.47216191131493</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -6049,19 +6049,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0540057686841356</v>
+        <v>0.03184084281089725</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1511754601520262</v>
+        <v>0.1468975787836912</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>1.88872643701646</v>
+        <v>0.3841230597408987</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2323914126729635</v>
+        <v>0.1784400258095062</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>31.11276439297789</v>
+        <v>28.47216191131494</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -6407,23 +6407,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.07658944853943661</v>
+        <v>0.01933473853886255</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1836325582950724</v>
+        <v>0.101642312937694</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>2.111356614395695</v>
+        <v>0.3393509756479683</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2767479874171384</v>
+        <v>0.1390494104225636</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>35.17816215304095</v>
+        <v>20.48025584607545</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -6437,23 +6437,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.06781823804752642</v>
+        <v>0.01933473853886255</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1740234267735215</v>
+        <v>0.101642312937694</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>2.032546691935583</v>
+        <v>0.3393509756479683</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2604193503707557</v>
+        <v>0.1390494104225636</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>34.05757964138278</v>
+        <v>20.48025584607544</v>
       </c>
     </row>
     <row r="14">
@@ -6469,23 +6469,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.1224532457992562</v>
+        <v>0.05196560514947892</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2621478076738443</v>
+        <v>0.1930037380352634</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>2.478834434272046</v>
+        <v>0.5356585730610701</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.3499332019103877</v>
+        <v>0.2279596568462914</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>44.5913337586386</v>
+        <v>35.1819599379021</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -6499,23 +6499,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.06625620407784365</v>
+        <v>0.05196560514947892</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1912670368644265</v>
+        <v>0.1930037380352634</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>1.902746508453199</v>
+        <v>0.5356585730610701</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2574028051087316</v>
+        <v>0.2279596568462914</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>37.13298713854047</v>
+        <v>35.1819599379021</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -6535,19 +6535,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.07029207665536839</v>
+        <v>0.01812511185111198</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1801813615570076</v>
+        <v>0.101839714647801</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>2.060440814210106</v>
+        <v>0.3115073985042406</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2651265295200924</v>
+        <v>0.134629535582323</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>34.97521956657769</v>
+        <v>21.52126607396653</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -6561,23 +6561,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.06650399354369461</v>
+        <v>0.01812511185111198</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1771561910911542</v>
+        <v>0.101839714647801</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>1.973786814179334</v>
+        <v>0.3115073985042406</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2578836821974097</v>
+        <v>0.134629535582323</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>33.86364488626052</v>
+        <v>21.52126607396653</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -7329,19 +7329,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.07541253140229112</v>
+        <v>0.04587074277737554</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2131303619045989</v>
+        <v>0.1661548067431136</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>2.089788283037184</v>
+        <v>0.5583632710273708</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2746134217446247</v>
+        <v>0.2141745614618495</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>40.61216297958273</v>
+        <v>30.43555137849643</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -7359,19 +7359,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.07186786390778678</v>
+        <v>0.04364069011158772</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2027079846486918</v>
+        <v>0.1641931102090178</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>2.073736593213498</v>
+        <v>0.5255106246524344</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2680818231581298</v>
+        <v>0.2089035426018135</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>39.07102625055413</v>
+        <v>30.08504662285747</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -7717,23 +7717,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.08331745920140109</v>
+        <v>0.04420897831616233</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.2130444756446578</v>
+        <v>0.1718093599316276</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>2.297047527091737</v>
+        <v>0.5707982254146486</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2886476384822871</v>
+        <v>0.2102593120795422</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>39.86850006686368</v>
+        <v>31.90960396473914</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -7747,23 +7747,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.07753774006204009</v>
+        <v>0.04139314964336322</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.2031942495939582</v>
+        <v>0.1588820664232643</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>2.160433573233221</v>
+        <v>0.5042238913073109</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2784559930438562</v>
+        <v>0.2034530649642891</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>38.80437063211963</v>
+        <v>29.88588481087761</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -7783,19 +7783,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.07340378738298402</v>
+        <v>0.06363324400212854</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2136019639138902</v>
+        <v>0.2059456431235465</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>2.012528948091113</v>
+        <v>0.7012246007221211</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2709313333355594</v>
+        <v>0.2522563061691988</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>40.96287854613907</v>
+        <v>36.69178283763069</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -7809,23 +7809,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.1436427006555076</v>
+        <v>0.050653591410671</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.3300838583814666</v>
+        <v>0.1769784706608509</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>1.364317663602063</v>
+        <v>0.6219403695765355</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.3790022436022082</v>
+        <v>0.2250635274998395</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>67.71837450046445</v>
+        <v>32.22995919970621</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -7841,23 +7841,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.09738206773070372</v>
+        <v>0.04780596162352267</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2207523619490231</v>
+        <v>0.175262941512984</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>2.391916671109531</v>
+        <v>0.6110860397465147</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.3120610000155478</v>
+        <v>0.2186457445813265</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>41.25747255073131</v>
+        <v>32.97380312588118</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -7871,23 +7871,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.08417538293233476</v>
+        <v>0.04166313485695962</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2164998312154916</v>
+        <v>0.1582405185959954</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>2.124231865072725</v>
+        <v>0.5395936572609777</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2901299414612955</v>
+        <v>0.204115493916948</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>40.82262909971556</v>
+        <v>30.28159976743834</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -8639,19 +8639,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.06717594464735673</v>
+        <v>0.03424918748467441</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2021563578971377</v>
+        <v>0.1388181449869916</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.961348933574598</v>
+        <v>0.5076784994596062</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2591832260146415</v>
+        <v>0.1850653600344332</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>39.26785737171992</v>
+        <v>26.09948093979845</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -8669,19 +8669,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.06743133069014497</v>
+        <v>0.0363076630032729</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2035779431588939</v>
+        <v>0.144988335171933</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>1.971283751612623</v>
+        <v>0.5319214573795747</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.259675433358924</v>
+        <v>0.190545697939557</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>39.43004934087699</v>
+        <v>27.70520785118033</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -9027,23 +9027,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.07634143097434205</v>
+        <v>0.02529602916804123</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.2139347887987639</v>
+        <v>0.1222137374809249</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>2.160660145437312</v>
+        <v>0.4650906347094994</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2762995312597219</v>
+        <v>0.159047254512743</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>40.32254738482865</v>
+        <v>25.04602975333767</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -9057,23 +9057,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.07413950795532617</v>
+        <v>0.02676622564259604</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.215140274785876</v>
+        <v>0.1263931029625702</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>2.103845714710497</v>
+        <v>0.4871184278788774</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2722857101563102</v>
+        <v>0.1636038680551167</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>40.72580064890713</v>
+        <v>25.881289330407</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -9089,23 +9089,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.06995461676491495</v>
+        <v>0.06171902017193677</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2131863741326089</v>
+        <v>0.1876822270920952</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1.580387815954285</v>
+        <v>0.7876774974131515</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.264489350948039</v>
+        <v>0.2484331301818193</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>42.52535622256002</v>
+        <v>34.09579750133805</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -9119,23 +9119,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.1131953429214891</v>
+        <v>0.06590592302438278</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2786903278678595</v>
+        <v>0.2081079328774631</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>1.285367523319278</v>
+        <v>0.7577970869794819</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.3364451558894689</v>
+        <v>0.256721489214251</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>58.44028041831636</v>
+        <v>37.74542505631312</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -9155,19 +9155,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.07043425996046698</v>
+        <v>0.06743289983958836</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2088867162169205</v>
+        <v>0.2088630141356293</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>2.036212146908684</v>
+        <v>0.7530095870444297</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2653945364178905</v>
+        <v>0.2596784547081031</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>39.99898901902026</v>
+        <v>37.89204751497597</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -9181,23 +9181,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.07043425996046698</v>
+        <v>0.02736888734697313</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2088867162169205</v>
+        <v>0.1289473103453577</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>2.036212146908684</v>
+        <v>0.4517390361501645</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2653945364178905</v>
+        <v>0.1654354476736263</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>39.99898901902026</v>
+        <v>28.06316840126037</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -9949,19 +9949,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.6264992793819176</v>
+        <v>0.2215938177227007</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.4045412171545907</v>
+        <v>0.367369878990759</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.5853643097759653</v>
+        <v>0.1991742118674624</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.7915170745991003</v>
+        <v>0.4707375252969543</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>20.60411308926322</v>
+        <v>17.31241443814804</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -9979,19 +9979,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.6565317710311874</v>
+        <v>0.270005917491776</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.3937141513635121</v>
+        <v>0.427934467354557</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.6020534974525554</v>
+        <v>0.2108792030463973</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.8102664814930872</v>
+        <v>0.519620936348581</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>20.15536972263859</v>
+        <v>19.65734158826409</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -10341,19 +10341,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.6623843702288218</v>
+        <v>0.2506710200927215</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.3906956676037835</v>
+        <v>0.3351387440057465</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.603008042405523</v>
+        <v>0.1998614408859472</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.8138699959015702</v>
+        <v>0.5006705704280225</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>19.99741797200817</v>
+        <v>15.97231778422038</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -10367,23 +10367,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.6443917535924693</v>
+        <v>0.3446595553841078</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.3814107009804614</v>
+        <v>0.393249393832188</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.5959123293708292</v>
+        <v>0.1996179861006587</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.8027401532204984</v>
+        <v>0.5870771289908233</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>19.4611078823345</v>
+        <v>18.73063970073006</v>
       </c>
     </row>
     <row r="14">
@@ -10403,19 +10403,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.6142914718091105</v>
+        <v>0.3388007269921566</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.4552426274651957</v>
+        <v>0.3283859391798689</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.587036179104248</v>
+        <v>0.2579376173549496</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.7837674858075643</v>
+        <v>0.5820659129275281</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>22.728390221047</v>
+        <v>15.03769294600273</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -10429,23 +10429,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.724042011466158</v>
+        <v>0.2897780061853846</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.471546147832866</v>
+        <v>0.3045188616623521</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.6333578339484077</v>
+        <v>0.2376590583639613</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.8509065821029698</v>
+        <v>0.5383103251706999</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>23.12695736201627</v>
+        <v>14.21146244842424</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -10461,23 +10461,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.63595040237567</v>
+        <v>0.3223637308523791</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.4329166600706871</v>
+        <v>0.4340856039700473</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.6080079217702899</v>
+        <v>0.2567695770302077</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.7974649850467856</v>
+        <v>0.5677708436089151</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>21.94459175025931</v>
+        <v>19.48461973596336</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -10491,23 +10491,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.7551301700693759</v>
+        <v>0.3150394120013743</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.4836793257148434</v>
+        <v>0.4247254807055391</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.6497653646142139</v>
+        <v>0.2347743160806917</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.8689822610786574</v>
+        <v>0.5612837179193552</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>23.35806702131448</v>
+        <v>19.34849266041439</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -11259,19 +11259,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.5994467069689204</v>
+        <v>0.2941975215742318</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.3810138289765668</v>
+        <v>0.4023307574181507</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.5951663634624212</v>
+        <v>0.2445628709403092</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.7742394377509586</v>
+        <v>0.5423997802121898</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>19.76439599489068</v>
+        <v>18.79600024155648</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -11289,19 +11289,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.5973125293566621</v>
+        <v>0.2786823554839949</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.3674352182092439</v>
+        <v>0.4183320297543201</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.5881225455384488</v>
+        <v>0.2263259317358666</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.7728599674951874</v>
+        <v>0.5279037369483142</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>19.22722356065988</v>
+        <v>19.31918095722702</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -11651,19 +11651,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.5199829564961943</v>
+        <v>0.2422181211485887</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.3553396967908581</v>
+        <v>0.3271912475227701</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.5234795423437058</v>
+        <v>0.229401185141675</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.7210984374523317</v>
+        <v>0.4921566022604885</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>19.47184159418081</v>
+        <v>15.78040335871052</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -11681,19 +11681,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.515685847951719</v>
+        <v>0.2767337333858051</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.3487325895839731</v>
+        <v>0.3756341033180781</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.5137916704409113</v>
+        <v>0.200699108801324</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.7181126986425731</v>
+        <v>0.5260548767816957</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>19.23509600640053</v>
+        <v>18.413060624853</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -11709,53 +11709,53 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.9054709335396565</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.6609884106464093</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.402675241320736</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.9515623645035866</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>31.91753779043063</v>
+      </c>
+      <c r="I14" s="9" t="inlineStr">
+        <is>
+          <t>Stacking Regressor</t>
+        </is>
+      </c>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
           <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
-      <c r="D14" s="5" t="n">
-        <v>0.6152738051237669</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>0.3800349338395541</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0.5978325495735759</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>0.7843939094127178</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>20.09840198380451</v>
-      </c>
-      <c r="I14" s="9" t="inlineStr">
-        <is>
-          <t>Stacking Regressor</t>
-        </is>
-      </c>
-      <c r="J14" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K14" s="8" t="inlineStr">
-        <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
-        </is>
-      </c>
       <c r="L14" s="8" t="n">
-        <v>0.7437767869860594</v>
+        <v>0.2839345693539689</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.5516084848548559</v>
+        <v>0.3579881156395073</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.6321979164501226</v>
+        <v>0.2614422501244869</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.8624249457118338</v>
+        <v>0.5328551110329796</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>26.80785044898454</v>
+        <v>17.20889345589081</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -11771,23 +11771,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.6081703988766763</v>
+        <v>0.3577719211416653</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.460584758893104</v>
+        <v>0.4556692778119775</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.5704363510404585</v>
+        <v>0.289680765880828</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.7798528059042145</v>
+        <v>0.5981403858139536</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>23.55050848209836</v>
+        <v>20.6843751649062</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -11801,23 +11801,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.6127358797280847</v>
+        <v>0.3329194799120329</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.4417907242068257</v>
+        <v>0.4557383089980693</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.5775137560961782</v>
+        <v>0.2740192915132898</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.7827744756493308</v>
+        <v>0.5769917502980723</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>22.73293363931115</v>
+        <v>20.83224862119262</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -12569,19 +12569,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.6330179148535452</v>
+        <v>0.3312668700383365</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.401348343864633</v>
+        <v>0.441255247766859</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.3405782660575119</v>
+        <v>0.2820959735978104</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.7956242296797812</v>
+        <v>0.5755578772272485</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>20.38175206685644</v>
+        <v>20.97513857924604</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -12599,19 +12599,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.6927410636102999</v>
+        <v>0.338441834316056</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.4254319095877765</v>
+        <v>0.4531988061029664</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.366889964169078</v>
+        <v>0.2675191802035822</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.8323106773376753</v>
+        <v>0.5817575391140677</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>21.42062809460828</v>
+        <v>21.63683711419956</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -12961,19 +12961,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.5643421241560475</v>
+        <v>0.3777632779954267</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.3497149727479014</v>
+        <v>0.4744828570582029</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.3097367454425244</v>
+        <v>0.2948926691837723</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.7512270789555229</v>
+        <v>0.6146245016230859</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>18.62598716423051</v>
+        <v>23.13353374854344</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -12991,19 +12991,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.631225350042227</v>
+        <v>0.3343143690115136</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.3697491614035309</v>
+        <v>0.4388840473232029</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.3309670495449685</v>
+        <v>0.2709644164004866</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.7944969163201497</v>
+        <v>0.578199246809881</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>19.32856265786406</v>
+        <v>21.18707714497218</v>
       </c>
     </row>
     <row r="14">
@@ -13023,19 +13023,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.7075008395485363</v>
+        <v>0.3494769459340011</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.3811222131197788</v>
+        <v>0.3645533969503947</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.3617510667029255</v>
+        <v>0.3243263277258994</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.8411306911226912</v>
+        <v>0.5911657516585354</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>19.3147887084238</v>
+        <v>17.68936475202754</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -13053,19 +13053,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.8169821383699789</v>
+        <v>0.3313241991195432</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.4225167677522932</v>
+        <v>0.3900873710524339</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.3952553890082091</v>
+        <v>0.3151712541804327</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.9038706424981281</v>
+        <v>0.5756076781276838</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>20.50589126830364</v>
+        <v>18.80019877460239</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -13081,23 +13081,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.6651237723516568</v>
+        <v>0.4100044154044259</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.4906082053249829</v>
+        <v>0.5059683182019513</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.3638523343964614</v>
+        <v>0.3343456063962562</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.815551207682054</v>
+        <v>0.6403158715855994</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>25.04364644519689</v>
+        <v>23.67987875456881</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -13111,23 +13111,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.7775381767911175</v>
+        <v>0.3948739368986153</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.4906458020399134</v>
+        <v>0.5141669477295173</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.3791778148769429</v>
+        <v>0.3275705506536701</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.8817812522338618</v>
+        <v>0.6283899560771283</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>24.37178862781658</v>
+        <v>24.10969292498979</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -13879,19 +13879,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.1502275699454174</v>
+        <v>0.0833681214942745</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2943199755934419</v>
+        <v>0.2455286285769241</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.4628597682625418</v>
+        <v>0.6046343167427159</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.3875920148112153</v>
+        <v>0.2887353831699096</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>42.36572963785169</v>
+        <v>40.80262388757102</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -14177,23 +14177,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 200}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.05585033387570495</v>
+        <v>0.02335392833350097</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1963673567643169</v>
+        <v>0.1250218180228647</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.3017468198205178</v>
+        <v>0.3463423136778397</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2363267523487448</v>
+        <v>0.1528199212586532</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>32.5764379464436</v>
+        <v>24.39291800498536</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -14221,23 +14221,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.02602090667160988</v>
+        <v>0.1018252104997111</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1295965044576265</v>
+        <v>0.2247666517786862</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.2538264755657613</v>
+        <v>0.5905842108608048</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.1613099707755534</v>
+        <v>0.3191006275451541</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>20.85541841608295</v>
+        <v>41.72097997131771</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -14269,19 +14269,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.04099572995453754</v>
+        <v>0.03728899401951286</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1664311730998728</v>
+        <v>0.1512034469186858</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.291775457910137</v>
+        <v>0.481449743853078</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2024740229129098</v>
+        <v>0.1931035836526936</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>27.2770782836816</v>
+        <v>27.92649945299864</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -14901,19 +14901,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0882357193533642</v>
+        <v>0.0296938965498768</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2378669898062115</v>
+        <v>0.136426658780902</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.7157948687450293</v>
+        <v>0.3586887734040594</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2970449786705108</v>
+        <v>0.172319170581444</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>41.037359426122</v>
+        <v>25.25504809747598</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -14931,19 +14931,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.09080790819426705</v>
+        <v>0.03214478322514232</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2377471411056986</v>
+        <v>0.1432213476419001</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.8100555804889321</v>
+        <v>0.3371090360595724</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.3013435053129021</v>
+        <v>0.1792896629065444</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>39.86180469374</v>
+        <v>27.85190484150617</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -15289,23 +15289,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.07764919526711218</v>
+        <v>0.02228037523004354</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.2163573338041818</v>
+        <v>0.1165485216146087</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.6988250327003555</v>
+        <v>0.3807874845346003</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2786560519118725</v>
+        <v>0.1492661221779528</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>37.05005633889694</v>
+        <v>23.34162567589575</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -15319,23 +15319,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 200}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.07580105542521469</v>
+        <v>0.02253865766972281</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.2092742559840365</v>
+        <v>0.1189211259363291</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.7241912931799596</v>
+        <v>0.3668349159600738</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2753199146905554</v>
+        <v>0.1501288035978533</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>35.44650679933994</v>
+        <v>23.54191955563868</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -15351,23 +15351,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.1122487801423886</v>
+        <v>0.04254843487141838</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2621057672423709</v>
+        <v>0.1596267101205738</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.5222479845847555</v>
+        <v>0.6440998637878655</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.3350354908698309</v>
+        <v>0.2062727196490568</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>52.4194269081152</v>
+        <v>30.57069895966758</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -15381,23 +15381,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.08384538057359517</v>
+        <v>0.1747848188236796</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2368876311030566</v>
+        <v>0.3402352908010962</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.4934571830090068</v>
+        <v>0.8945924312398483</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2895606682089181</v>
+        <v>0.4180727434594124</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>42.9137666700659</v>
+        <v>65.41387972605162</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -15413,23 +15413,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.06436263083206335</v>
+        <v>0.03667708656356015</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2024447270536349</v>
+        <v>0.1505544271801755</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.6147466144747596</v>
+        <v>0.4983706851966447</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2536979125496766</v>
+        <v>0.1915126276869495</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>34.98042100446048</v>
+        <v>28.92782363273438</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -15443,23 +15443,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.06436263083206335</v>
+        <v>0.03986238194598953</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2024447270536349</v>
+        <v>0.1556066064847781</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.6147466144747596</v>
+        <v>0.5424474534488121</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2536979125496766</v>
+        <v>0.1996556584371941</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>34.98042100446048</v>
+        <v>29.77771183086448</v>
       </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
@@ -16211,19 +16211,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.06568417156976677</v>
+        <v>0.2663926103264924</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2025734650766995</v>
+        <v>0.4151244794271223</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.480636906323379</v>
+        <v>1.229212649843141</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2562892342057441</v>
+        <v>0.5161323573721108</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>37.35781960272928</v>
+        <v>67.42104326505603</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -16509,23 +16509,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.04474526110488306</v>
+        <v>0.07568992439314536</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1640483354530301</v>
+        <v>0.2268252393145097</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.4407038072839</v>
+        <v>0.7968487726459724</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2115307568768265</v>
+        <v>0.2751180190266449</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>27.86467872600065</v>
+        <v>45.53786810935313</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -16557,19 +16557,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.08876203820092388</v>
+        <v>0.1135978788080168</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2491170168498955</v>
+        <v>0.2626556026941634</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.5608063440561529</v>
+        <v>0.8256884589795078</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2979295859778345</v>
+        <v>0.3370428441726909</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>42.54672259027149</v>
+        <v>45.2456961228377</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -16597,23 +16597,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.05708941448535501</v>
+        <v>0.05842584729152771</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1903011716057363</v>
+        <v>0.1872467969493899</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.494304436956267</v>
+        <v>0.6870200556885124</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2389339123802961</v>
+        <v>0.2417143919826201</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>31.93583952126601</v>
+        <v>33.23467012463409</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -17233,19 +17233,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.1359834276181834</v>
+        <v>14.51666799220296</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2885270318605755</v>
+        <v>3.113347716089639</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.8134563064502319</v>
+        <v>7.857181860905539</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.3687593085173355</v>
+        <v>3.81007453893004</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>51.36138318145682</v>
+        <v>164.3136703490709</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -17535,19 +17535,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.089445687059867</v>
+        <v>1.698185570112965</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.2395704078995859</v>
+        <v>1.07055058411763</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.666842311903317</v>
+        <v>2.427044193244014</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2990747181890622</v>
+        <v>1.303144493182918</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>41.97543080711509</v>
+        <v>128.9973857993222</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -17579,19 +17579,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.07000791212826356</v>
+        <v>0.03585355510185968</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2055965801388561</v>
+        <v>0.1489585229416201</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.6931945092932621</v>
+        <v>0.5456309383044584</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2645900832009083</v>
+        <v>0.1893503501498207</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>35.30964133252468</v>
+        <v>29.09386909585842</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -17623,19 +17623,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.06436263083206335</v>
+        <v>0.06743289983958836</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2024447270536349</v>
+        <v>0.2088630141356293</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.6147466144747596</v>
+        <v>0.7530095870444297</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2536979125496766</v>
+        <v>0.2596784547081031</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>34.98042100446048</v>
+        <v>37.89204751497597</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -18255,19 +18255,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.8763753345067269</v>
+        <v>1.801893304477937</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.7471345299622558</v>
+        <v>1.130808340575753</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.3029155307416733</v>
+        <v>0.441797440094829</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.9361492052588235</v>
+        <v>1.342346193974541</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>30.89955978885209</v>
+        <v>48.96819438851954</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -18553,23 +18553,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.9866992791368985</v>
+        <v>0.7883049447037811</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.7933702974170666</v>
+        <v>0.6676089916128682</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.3140172680388629</v>
+        <v>0.2964611579502411</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.9933273776237613</v>
+        <v>0.8878653865895331</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>41.8965790905962</v>
+        <v>32.90448098227537</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -18601,19 +18601,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.1517020455226395</v>
+        <v>0.2672460193000062</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2701461291821238</v>
+        <v>0.2864126836802448</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1262948069856061</v>
+        <v>0.2292071158143086</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.3894894677942389</v>
+        <v>0.5169584309207136</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>10.6760298652303</v>
+        <v>13.54558692074163</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -18645,19 +18645,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.2189462469363219</v>
+        <v>0.3479052990335734</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3724644478340365</v>
+        <v>0.4696631994164505</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.1520561934910422</v>
+        <v>0.2683412610434247</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.4679169231138385</v>
+        <v>0.5898349761022768</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>14.79142500838071</v>
+        <v>20.93790420851168</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -19277,19 +19277,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.254934029011807</v>
+        <v>7.133884150090665</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.8577830568367998</v>
+        <v>2.273695446272032</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.3326557294302513</v>
+        <v>1.058154462164375</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.120238380440434</v>
+        <v>2.670933198357957</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>32.14040464405799</v>
+        <v>113.6124205755863</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -19575,23 +19575,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.6903712513455025</v>
+        <v>2.174334588147904</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.6513554154122719</v>
+        <v>1.240035824891732</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.2460048055107659</v>
+        <v>0.5111645654836319</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.8308858232907229</v>
+        <v>1.474562507372239</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>28.99372247338612</v>
+        <v>71.56148256348477</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -19623,19 +19623,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.207499356700652</v>
+        <v>0.5452061214976243</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2753549741832928</v>
+        <v>0.4757295566156433</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1810223324801555</v>
+        <v>0.3571324620437877</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.4555209728438988</v>
+        <v>0.7383807429081721</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>12.16896259101762</v>
+        <v>19.90975655355236</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -19663,23 +19663,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.3759132465284691</v>
+        <v>0.3871718462145072</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.5159619721567326</v>
+        <v>0.4933880289172954</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2400590703548713</v>
+        <v>0.3042589580433174</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.613117644933229</v>
+        <v>0.6222313446094685</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>22.11215907857711</v>
+        <v>22.27358445898558</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -20299,19 +20299,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>11.46468190560617</v>
+        <v>16.8256562677508</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>2.692986870247274</v>
+        <v>3.034096719973165</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.196222279861066</v>
+        <v>1.555846529653514</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>3.385953618348334</v>
+        <v>4.101908856587479</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>105.2737273302539</v>
+        <v>86.48841299363201</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -20597,23 +20597,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>2.038895981651102</v>
+        <v>2.331216566064049</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>1.135323454224069</v>
+        <v>1.129125068071288</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.4456807970394208</v>
+        <v>0.595056916257735</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>1.427899149677981</v>
+        <v>1.526832199707633</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>59.82666687187569</v>
+        <v>50.92755744588449</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -20645,19 +20645,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.3222916843528218</v>
+        <v>0.3575090159690998</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.336036784114378</v>
+        <v>0.3524693083373573</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.2547893596803958</v>
+        <v>0.3245109688001093</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.5677073932518598</v>
+        <v>0.5979205766396569</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>15.23028918190462</v>
+        <v>17.25183407831085</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -20685,23 +20685,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.708345582588122</v>
+        <v>0.4419534790773146</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.717716393145399</v>
+        <v>0.5310330231267237</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.3209690672490538</v>
+        <v>0.3644527833355158</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.8416326886404317</v>
+        <v>0.664795817584102</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>33.31232193251545</v>
+        <v>24.51642364122767</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -21321,19 +21321,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.04534230641426309</v>
+        <v>0.06532149530878857</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1621337512339186</v>
+        <v>0.2082116877818946</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.4595424425328608</v>
+        <v>0.6050028756289358</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2129373297810017</v>
+        <v>0.255580702144721</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>27.38042013840942</v>
+        <v>38.31451530562271</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -21351,19 +21351,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.05316341110232915</v>
+        <v>0.06731697983819322</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1687058832479008</v>
+        <v>0.2096975483136838</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.4674020626284484</v>
+        <v>0.5985804414233362</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2305719217561608</v>
+        <v>0.2594551595906183</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>27.89188850534563</v>
+        <v>38.19756906198396</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -21709,23 +21709,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.0405025595835332</v>
+        <v>0.04653108545089726</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.151579797346281</v>
+        <v>0.1632676087307852</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.4614225436338039</v>
+        <v>0.6216787891992471</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2012524772109233</v>
+        <v>0.2157106521498121</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>26.13033379968424</v>
+        <v>30.1085294181043</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -21739,23 +21739,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.04387348815433337</v>
+        <v>0.04522497955563991</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1555438957396494</v>
+        <v>0.1601285509042676</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.4657200181143785</v>
+        <v>0.6140884557688674</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2094599917748814</v>
+        <v>0.2126616551135627</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>26.69294726657307</v>
+        <v>29.15850623942864</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -21775,19 +21775,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.0661087711433723</v>
+        <v>0.06442973585108012</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2059298380635033</v>
+        <v>0.206452935970866</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.5263818145242865</v>
+        <v>0.6553530127254947</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2571162599746898</v>
+        <v>0.2538301318816978</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>34.40221937299917</v>
+        <v>37.07460039962677</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -21805,19 +21805,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.06855451411997011</v>
+        <v>0.07048270072257584</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2115918254958882</v>
+        <v>0.2174824303883045</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.5237289108807859</v>
+        <v>0.7139267160197255</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2618291697270763</v>
+        <v>0.2654857825243677</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>35.48936984870322</v>
+        <v>38.29663649658854</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -21833,23 +21833,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.04373019814954225</v>
+        <v>0.05295022833389149</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1681977594214826</v>
+        <v>0.1726870262117264</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.4994957172115681</v>
+        <v>0.7027129603962788</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2091176657997651</v>
+        <v>0.2301091661231501</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>28.48918849925052</v>
+        <v>31.49930265285497</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -21867,19 +21867,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.04585944320313545</v>
+        <v>0.04612271943940776</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.169848413449799</v>
+        <v>0.1595681405329601</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.501199014067859</v>
+        <v>0.6227847221226778</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2141481804805622</v>
+        <v>0.2147620065081526</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>28.69107725816247</v>
+        <v>30.13856003710292</v>
       </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
@@ -22631,19 +22631,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.2090230231483232</v>
+        <v>0.2036154351235087</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.3970740304390543</v>
+        <v>0.3832986326570061</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1545173821893598</v>
+        <v>0.1591063036164318</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.4571903576720787</v>
+        <v>0.4512376703285185</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>17.24629873988339</v>
+        <v>16.76850551789959</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -22661,19 +22661,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.1702762931317764</v>
+        <v>0.1961817891651741</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.3625881271860286</v>
+        <v>0.3701394400259072</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1401344952880604</v>
+        <v>0.151088074049473</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.4126454811721272</v>
+        <v>0.4429241347738618</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>15.45535485454588</v>
+        <v>16.64474252468406</v>
       </c>
     </row>
     <row r="8" ht="28.5" customHeight="1">
@@ -23023,19 +23023,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.08148066264742652</v>
+        <v>0.1431760449432278</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.2493928929643696</v>
+        <v>0.2914289458214778</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1019118388521898</v>
+        <v>0.1783973786008747</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2854481785673654</v>
+        <v>0.3783861056424083</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>10.13335527390794</v>
+        <v>14.09827965874686</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -23053,19 +23053,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.07528709703614346</v>
+        <v>0.146401567531303</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.2353051446995849</v>
+        <v>0.2985638183931719</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.09507639036690932</v>
+        <v>0.1688738012108826</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2743849431658805</v>
+        <v>0.3826245777930412</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>9.506283895564692</v>
+        <v>14.2969967589924</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -23085,19 +23085,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.130522177964542</v>
+        <v>0.2930479167743428</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2337920567770494</v>
+        <v>0.2739604838579124</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1071377067696054</v>
+        <v>0.2308461238916246</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.3612785323881589</v>
+        <v>0.5413390035590848</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>9.399469641773553</v>
+        <v>13.03663786172566</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -23115,19 +23115,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.1268137279194322</v>
+        <v>0.2493023717694889</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2451307001953667</v>
+        <v>0.2746045652983226</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.1074280300136011</v>
+        <v>0.2162736624325945</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.3561091516928935</v>
+        <v>0.4993018844041037</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>9.837752906320588</v>
+        <v>13.13356812249692</v>
       </c>
     </row>
     <row r="15" ht="42.75" customHeight="1">
@@ -23143,23 +23143,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.08716303429944623</v>
+        <v>0.1716165540549237</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2195611132728897</v>
+        <v>0.2916856229760862</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.09071119415569961</v>
+        <v>0.1817689100740957</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2952338637410116</v>
+        <v>0.4142662839948765</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>8.89661031746431</v>
+        <v>14.6400285302052</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -23173,23 +23173,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.1788103844459114</v>
+        <v>0.2648665343115745</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.3303688356707087</v>
+        <v>0.3386854933437647</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.1344860761754734</v>
+        <v>0.2220218468320646</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.4228597692449725</v>
+        <v>0.5146518573866945</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>13.09919653731204</v>
+        <v>16.01485623723057</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -23942,19 +23942,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.3426649786612618</v>
+        <v>0.4136990244977201</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.4946331477450602</v>
+        <v>0.5206613176682703</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.2332009535293993</v>
+        <v>0.2663320789735504</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.5853759293490481</v>
+        <v>0.6431943909097156</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>22.39052901432541</v>
+        <v>24.50587850415762</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -23972,19 +23972,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.3327242215779194</v>
+        <v>0.3654543085789429</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.4772389041703947</v>
+        <v>0.4779940628236844</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.2272115595718255</v>
+        <v>0.235653659576923</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.5768225217325684</v>
+        <v>0.6045281702112342</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>21.77912061887885</v>
+        <v>24.00084039555216</v>
       </c>
     </row>
     <row r="8" ht="28.5" customHeight="1">
@@ -24330,23 +24330,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.1714117507302845</v>
+        <v>0.2287607832011662</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.3062016287260386</v>
+        <v>0.3244373924511778</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1884696833268988</v>
+        <v>0.2544380324805006</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.4140190221841075</v>
+        <v>0.4782894345489624</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>14.17037131289796</v>
+        <v>15.80500157345551</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -24364,19 +24364,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.1743969653287109</v>
+        <v>0.2180542482176686</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.300438722523684</v>
+        <v>0.3191212204158083</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.1929567176993543</v>
+        <v>0.2450246511146788</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.4176086269807065</v>
+        <v>0.4669627910419294</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>14.08813212771124</v>
+        <v>15.8187732797957</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -24396,19 +24396,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.2781015046881249</v>
+        <v>0.3201404553201103</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2949910679622967</v>
+        <v>0.3282408848748538</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.232944344933334</v>
+        <v>0.3067249649937003</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.527353301580757</v>
+        <v>0.5658095574662116</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>13.81362418316913</v>
+        <v>16.3359571225656</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -24426,19 +24426,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.264211112439818</v>
+        <v>0.2978692577186118</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.3079278080864799</v>
+        <v>0.3448486590918347</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.2316828562218222</v>
+        <v>0.2995609840233384</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.5140147006067219</v>
+        <v>0.5457739987564557</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>14.31590631411213</v>
+        <v>17.06028228959081</v>
       </c>
     </row>
     <row r="15" ht="42.75" customHeight="1">
@@ -24454,23 +24454,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.2645798481625638</v>
+        <v>0.2792114464279963</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3681864497092692</v>
+        <v>0.3276027224389718</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2177461221075478</v>
+        <v>0.2874343454117508</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.5143732576277307</v>
+        <v>0.5284046237761326</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>16.39008876029631</v>
+        <v>17.60282762996341</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -24484,23 +24484,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.2304243756355007</v>
+        <v>0.3365867747358342</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.3115088624520147</v>
+        <v>0.4272411154679255</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2211477567780046</v>
+        <v>0.3133089947735521</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.4800253906154347</v>
+        <v>0.5801609903602915</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>14.57129602434061</v>
+        <v>20.51042121491719</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -25253,19 +25253,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.2424703911525057</v>
+        <v>0.2059342858064432</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.4001932082525868</v>
+        <v>0.3510298065921394</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1744978310756146</v>
+        <v>0.1650773082638382</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.4924128259423242</v>
+        <v>0.4537998301084337</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>17.47781506045526</v>
+        <v>16.03208224141556</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -25283,19 +25283,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.2591470981712007</v>
+        <v>0.2911631515628085</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.4028420268567233</v>
+        <v>0.4045922075842562</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1670395434644102</v>
+        <v>0.1812100413870104</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.5090649253004972</v>
+        <v>0.5395953591005102</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>18.68747167131567</v>
+        <v>22.22450638497553</v>
       </c>
     </row>
     <row r="8" ht="28.5" customHeight="1">
@@ -25641,23 +25641,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.124345595883682</v>
+        <v>0.1318005175926538</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.2744465325772896</v>
+        <v>0.2355837490733358</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1414851526649196</v>
+        <v>0.1609726133442938</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.3526267089766202</v>
+        <v>0.3630434100664187</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>12.45415756708801</v>
+        <v>11.55266561255657</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -25675,19 +25675,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.1119415049263099</v>
+        <v>0.1206606157242546</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.2615722695038966</v>
+        <v>0.2430006165213937</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.1299568378319441</v>
+        <v>0.1494986903318231</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.3345766054677313</v>
+        <v>0.3473623694706359</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>11.90998069344183</v>
+        <v>11.90834321651717</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -25707,19 +25707,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.1629844319313273</v>
+        <v>0.3066756589342029</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2299172530707571</v>
+        <v>0.2990140664826184</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1561047494448432</v>
+        <v>0.2610650620912513</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.4037133041297095</v>
+        <v>0.5537830431985101</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>10.45967126561794</v>
+        <v>14.39906625926668</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -25737,19 +25737,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.1702855625269747</v>
+        <v>0.2640732160001952</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2239784621415352</v>
+        <v>0.3222409798419307</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.1596512940089139</v>
+        <v>0.2485343613226917</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.4126567126886156</v>
+        <v>0.5138805464309728</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>10.27323840712979</v>
+        <v>15.39499973987357</v>
       </c>
     </row>
     <row r="15" ht="42.75" customHeight="1">
@@ -25769,19 +25769,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.2589626554798626</v>
+        <v>0.2995696807190336</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3884523519917977</v>
+        <v>0.4306105580945346</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2036719049820907</v>
+        <v>0.2637243452440363</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.5088837347369854</v>
+        <v>0.5473295905750334</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>16.59505823285403</v>
+        <v>19.76198876094947</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -25795,23 +25795,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.2441172135372198</v>
+        <v>0.2859655406173229</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.3889050391858254</v>
+        <v>0.3876523552691364</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2034622214072825</v>
+        <v>0.2599228391587786</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.4940821930986987</v>
+        <v>0.5347574596182113</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>16.62787082453552</v>
+        <v>18.03122863155319</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -26566,19 +26566,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>9.787553797374864e-06</v>
+        <v>0.03096283416342742</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.002491760228787398</v>
+        <v>0.1394120719972438</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.004263607067471086</v>
+        <v>0.3926412984368913</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.003128506640135971</v>
+        <v>0.1759625930799709</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.4245645842575393</v>
+        <v>25.96816297631085</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -26596,19 +26596,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>9.546173097004827e-06</v>
+        <v>0.02698130731134824</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.002390611091569943</v>
+        <v>0.1313324402703953</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.004175668743454485</v>
+        <v>0.388220985691879</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.003089688187666326</v>
+        <v>0.1642598773631231</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.4155282870965178</v>
+        <v>25.25838130654257</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -26954,53 +26954,53 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
+          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 100}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.03356734105209101</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.1334486472471325</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.4287487482567794</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.1832139215564445</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>25.21946051625125</v>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>Voting Regressor</t>
+        </is>
+      </c>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
           <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
-      <c r="D13" s="5" t="n">
-        <v>0.03031952747787487</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>0.1392556064883088</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>0.1930290081584785</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <v>0.1741250340355311</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>20.93328153917856</v>
-      </c>
-      <c r="I13" s="9" t="inlineStr">
-        <is>
-          <t>Voting Regressor</t>
-        </is>
-      </c>
-      <c r="J13" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K13" s="8" t="inlineStr">
-        <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
-        </is>
-      </c>
       <c r="L13" s="8" t="n">
-        <v>0.02260913416130031</v>
+        <v>0.03726967329931929</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1185740165567534</v>
+        <v>0.1527384976154625</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2236029672101056</v>
+        <v>0.4551121006291449</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1503633404833117</v>
+        <v>0.1930535503411406</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>18.92903073422309</v>
+        <v>27.82257415584915</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -27016,23 +27016,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>2.316919878778751e-05</v>
+        <v>0.09097624556588836</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.004045501149636322</v>
+        <v>0.2416496092455689</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.006110417487085179</v>
+        <v>0.7958647162718451</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.004813439392761429</v>
+        <v>0.3016226874190474</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>0.6108823285447867</v>
+        <v>41.93437027748803</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -27046,23 +27046,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearRegression()}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.1041243736307793</v>
+        <v>0.09881707639981725</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2767859860325356</v>
+        <v>0.2512913460332361</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.595335344290141</v>
+        <v>0.8964850477652648</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.3226830854426356</v>
+        <v>0.3143518353689338</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>41.7911711207741</v>
+        <v>40.86012548172742</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -27078,23 +27078,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.0533224282163323</v>
+        <v>0.04429255731339809</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1816258351434023</v>
+        <v>0.1497443889474611</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.3453322867817593</v>
+        <v>0.5614243795607878</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.230916496197938</v>
+        <v>0.2104579704202197</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>28.34026631476321</v>
+        <v>26.99486664790601</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -27108,23 +27108,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0533224282163323</v>
+        <v>0.05846315396323661</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1816258351434023</v>
+        <v>0.1899874899891309</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.3453322867817593</v>
+        <v>0.6045655298949658</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.230916496197938</v>
+        <v>0.2417915506448408</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>28.34026631476321</v>
+        <v>33.43764838226924</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -27880,19 +27880,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.003065124719534096</v>
+        <v>0.04053926318004785</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.04434451047512875</v>
+        <v>0.1642201803150086</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1288197861496312</v>
+        <v>0.3520212881647435</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.05536356852239653</v>
+        <v>0.2013436444987719</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>10.25758990262414</v>
+        <v>30.28106947453775</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -27910,19 +27910,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0026218861569445</v>
+        <v>0.03996725298718251</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.04038195391203985</v>
+        <v>0.1648604664684444</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1121206415879072</v>
+        <v>0.3692081916795173</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.05120435681604155</v>
+        <v>0.199918115705362</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>9.211114416047057</v>
+        <v>30.4850187031463</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -28268,23 +28268,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.0439806623983476</v>
+        <v>0.05924049318659556</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1770153111247019</v>
+        <v>0.1984258994068804</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.3965585625338691</v>
+        <v>0.5292358748983436</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.209715670369068</v>
+        <v>0.2433936999731003</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>31.69227822667503</v>
+        <v>37.23190190683097</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -28298,23 +28298,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.0561863403526963</v>
+        <v>0.0748166758562443</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1999146386284857</v>
+        <v>0.2312926752401264</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2940126528286122</v>
+        <v>0.5120535609894353</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.237036580199547</v>
+        <v>0.2735263714091281</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>33.65480047708881</v>
+        <v>43.62218908404534</v>
       </c>
     </row>
     <row r="14">
@@ -28330,23 +28330,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': LinearRegression()}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.04125192519166989</v>
+        <v>0.5414918431654622</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1568991548818961</v>
+        <v>0.5465720773687889</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.5981979527891724</v>
+        <v>2.337506695092653</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.203105699554862</v>
+        <v>0.7358612934279545</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>28.4082964259823</v>
+        <v>71.47341450380654</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -28360,23 +28360,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.1048641004769491</v>
+        <v>0.08823819876998833</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2558160481890391</v>
+        <v>0.2196936990253568</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.9157001230866899</v>
+        <v>1.030870356713481</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.3238272695079109</v>
+        <v>0.2970491521112092</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>40.60364320785079</v>
+        <v>37.07081934684193</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -28396,19 +28396,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.06436263083206335</v>
+        <v>0.06743289983958836</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2024447270536349</v>
+        <v>0.2088630141356293</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.6147466144747596</v>
+        <v>0.7530095870444297</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2536979125496766</v>
+        <v>0.2596784547081031</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>34.98042100446048</v>
+        <v>37.89204751497597</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -28426,19 +28426,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.06436263083206335</v>
+        <v>0.06743289983958836</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2024447270536349</v>
+        <v>0.2088630141356293</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.6147466144747596</v>
+        <v>0.7530095870444297</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2536979125496766</v>
+        <v>0.2596784547081031</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>34.98042100446048</v>
+        <v>37.89204751497597</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -29192,19 +29192,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.02465383927808517</v>
+        <v>0.07401574815490175</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1154987153603183</v>
+        <v>0.2110708234872498</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.3182737770437604</v>
+        <v>0.6108305103164536</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.1570154109572852</v>
+        <v>0.2720583543192558</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>20.57770424586292</v>
+        <v>41.01926915596349</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -29222,19 +29222,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0252355609155453</v>
+        <v>0.07477753520396972</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1193112820686143</v>
+        <v>0.213833265598614</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.3291322408254562</v>
+        <v>0.6012982567338281</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1588570455332255</v>
+        <v>0.2734548138248251</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>21.32904450193384</v>
+        <v>40.85230670897639</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -29580,23 +29580,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.03714912507506971</v>
+        <v>0.05423559207280654</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1410119014599196</v>
+        <v>0.179141169426635</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.4062474543348581</v>
+        <v>0.6145618684365807</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1927410829975532</v>
+        <v>0.2328853625129895</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>24.26114716155877</v>
+        <v>32.66201915117997</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -29610,23 +29610,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.04143773132396043</v>
+        <v>0.05565955825058766</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1543331041624847</v>
+        <v>0.1839143303106919</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.4494810425740286</v>
+        <v>0.6118935159496764</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.203562598047776</v>
+        <v>0.2359227802705531</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>26.5551987486803</v>
+        <v>33.71727988452947</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -29642,53 +29642,53 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.07113650581625305</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.214439443216095</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.7029183307322608</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.2667142774885759</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>38.18359509716598</v>
+      </c>
+      <c r="I14" s="9" t="inlineStr">
+        <is>
+          <t>Stacking Regressor</t>
+        </is>
+      </c>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
           <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
-      <c r="D14" s="5" t="n">
-        <v>0.1155617949299559</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>0.2721291865914028</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0.5612895197618093</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>0.3399438114305891</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>50.3208533060799</v>
-      </c>
-      <c r="I14" s="9" t="inlineStr">
-        <is>
-          <t>Stacking Regressor</t>
-        </is>
-      </c>
-      <c r="J14" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K14" s="8" t="inlineStr">
-        <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
-        </is>
-      </c>
       <c r="L14" s="8" t="n">
-        <v>0.0953046868126817</v>
+        <v>0.1249314625704368</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2514466109706322</v>
+        <v>0.2831320874684012</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.6107011014936825</v>
+        <v>0.7335863380250691</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.3087145717530705</v>
+        <v>0.3534564507410167</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>42.38640401552583</v>
+        <v>54.60571833756784</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -29704,23 +29704,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.05708941448535501</v>
+        <v>0.06606488492420889</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1903011716057363</v>
+        <v>0.195504427955287</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.494304436956267</v>
+        <v>0.7996636994168668</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2389339123802961</v>
+        <v>0.2570309026638799</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>31.93583952126601</v>
+        <v>33.72821503944181</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -29734,23 +29734,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.05708941448535501</v>
+        <v>0.06054821712659977</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1903011716057363</v>
+        <v>0.1968028488520547</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.494304436956267</v>
+        <v>0.6577627012179064</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2389339123802961</v>
+        <v>0.2460654732517339</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>31.93583952126601</v>
+        <v>35.34839791535524</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">

</xml_diff>